<commit_message>
Adding additional labels, cleanup, and including the figure as JPG
</commit_message>
<xml_diff>
--- a/florida_examination.xlsx
+++ b/florida_examination.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Desktop\IDS-files\election conspiracy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Desktop\IDS-files\florida_git_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -275,7 +275,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -435,33 +435,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="6" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -472,7 +472,7 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -481,10 +481,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -495,8 +495,36 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFFF7575"/>
@@ -815,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -957,11 +985,11 @@
         <v>0.10785619174434088</v>
       </c>
       <c r="K3" s="29">
-        <f t="shared" ref="I3:K66" si="2">$B3-$E3</f>
+        <f t="shared" ref="K3:K66" si="2">$B3-$E3</f>
         <v>178.91100000000006</v>
       </c>
       <c r="L3" s="29">
-        <f t="shared" ref="J3:L66" si="3">$F3-$C3</f>
+        <f t="shared" ref="L3:L66" si="3">$F3-$C3</f>
         <v>1430.1049999999996</v>
       </c>
       <c r="M3" s="25"/>
@@ -3773,11 +3801,11 @@
         <v>0.1613262910798122</v>
       </c>
       <c r="K67" s="29">
-        <f t="shared" ref="I67:K68" si="6">$B67-$E67</f>
+        <f t="shared" ref="K67:K68" si="6">$B67-$E67</f>
         <v>-281.31999999999971</v>
       </c>
       <c r="L67" s="29">
-        <f t="shared" ref="J67:L68" si="7">$F67-$C67</f>
+        <f t="shared" ref="L67:L68" si="7">$F67-$C67</f>
         <v>4615.2799999999988</v>
       </c>
       <c r="M67" s="25"/>

</xml_diff>

<commit_message>
Added additional plot labels and results as JPG
</commit_message>
<xml_diff>
--- a/florida_examination.xlsx
+++ b/florida_examination.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Desktop\IDS-files\election conspiracy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Desktop\IDS-files\florida_git_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -275,7 +275,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -435,33 +435,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="6" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -472,7 +472,7 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -481,10 +481,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -495,8 +495,36 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFFF7575"/>
@@ -815,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -957,11 +985,11 @@
         <v>0.10785619174434088</v>
       </c>
       <c r="K3" s="29">
-        <f t="shared" ref="I3:K66" si="2">$B3-$E3</f>
+        <f t="shared" ref="K3:K66" si="2">$B3-$E3</f>
         <v>178.91100000000006</v>
       </c>
       <c r="L3" s="29">
-        <f t="shared" ref="J3:L66" si="3">$F3-$C3</f>
+        <f t="shared" ref="L3:L66" si="3">$F3-$C3</f>
         <v>1430.1049999999996</v>
       </c>
       <c r="M3" s="25"/>
@@ -3773,11 +3801,11 @@
         <v>0.1613262910798122</v>
       </c>
       <c r="K67" s="29">
-        <f t="shared" ref="I67:K68" si="6">$B67-$E67</f>
+        <f t="shared" ref="K67:K68" si="6">$B67-$E67</f>
         <v>-281.31999999999971</v>
       </c>
       <c r="L67" s="29">
-        <f t="shared" ref="J67:L68" si="7">$F67-$C67</f>
+        <f t="shared" ref="L67:L68" si="7">$F67-$C67</f>
         <v>4615.2799999999988</v>
       </c>
       <c r="M67" s="25"/>

</xml_diff>